<commit_message>
Added new class with location input
</commit_message>
<xml_diff>
--- a/target/classes/com/weather/excel/util/WeatherReportExcel.xlsx
+++ b/target/classes/com/weather/excel/util/WeatherReportExcel.xlsx
@@ -3,6 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
+  <mc:AlternateContent>
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shravyav\automation_WS\WhatsappWeatherReport\src\main\java\com\weather\excel\util\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16110" windowHeight="6120"/>
   </bookViews>
@@ -10,9 +15,8 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>UserName</t>
   </si>
@@ -37,11 +41,15 @@
 RealFeel® 33°
 Plenty of clouds</t>
   </si>
+  <si>
+    <t>https://api.whatsapp.com/send?phone=919542856170</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -80,7 +88,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -88,6 +96,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -370,28 +380,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="53.7109375" style="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="16384" width="9.140625" style="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" style="1" width="53.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="36.35546875" collapsed="true"/>
+    <col min="3" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" t="s" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -399,9 +409,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>